<commit_message>
Added three test cases about commas as decimal separators
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/Pham Hong Anh_Middle Assignment 1.xlsx
+++ b/Middle Assignment 1/Pham Hong Anh_Middle Assignment 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FF8D92-98A1-4B85-8EF0-79A8F546F0BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C10868A-86E1-43F6-85A1-FA6831E3EA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <author>ADMIN</author>
   </authors>
   <commentList>
-    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{49865CBD-780A-45DC-B325-3B9CCFE0DD01}">
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{49865CBD-780A-45DC-B325-3B9CCFE0DD01}">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Verify the correct display of currency</t>
   </si>
   <si>
-    <t>Verify that commas are used as decimal separators to display price</t>
-  </si>
-  <si>
     <t>Verify that the &lt;&gt; is in the correct size</t>
   </si>
   <si>
@@ -148,14 +145,23 @@
     <t>Verify the correct alignment of the price and product name</t>
   </si>
   <si>
-    <t>Verify that discounted price is rounded to the nearest integer using boundary value analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Case 1: The &lt; button can help users navigate to the previous photo but does not exceed the 1st photo
 - Case 2: The &gt; button can help users navigate to the next photo but does not exceed the 5th phot</t>
   </si>
   <si>
     <t>Verify that the &lt;&gt; button can help users navigate between photo using boundary value analysis with 2 boundary values of 1 and 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that discounted price is rounded to the nearest integer </t>
+  </si>
+  <si>
+    <t>Verify that commas are used as decimal separators to display price between ₫1,000 and ₫1,000,000</t>
+  </si>
+  <si>
+    <t>Verify that commas are used as decimal separators to display price between ₫0 and ₫1,000</t>
+  </si>
+  <si>
+    <t>Verify that commas are used as decimal separators to display price between ₫1,000 and ₫1,000,000,000</t>
   </si>
 </sst>
 </file>
@@ -597,10 +603,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -690,7 +696,7 @@
     </row>
     <row r="3" spans="1:26" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -752,7 +758,7 @@
     </row>
     <row r="5" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
-        <f t="shared" ref="A5:A12" ca="1" si="0">IF(OFFSET(A5,-1,0) ="",OFFSET(A5,-2,0)+1,OFFSET(A5,-1,0)+1 )</f>
+        <f t="shared" ref="A5:A14" ca="1" si="0">IF(OFFSET(A5,-1,0) ="",OFFSET(A5,-2,0)+1,OFFSET(A5,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -855,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -917,7 +923,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -945,12 +951,12 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>7</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -977,13 +983,13 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="A12:A13" ca="1" si="1">IF(OFFSET(A12,-1,0) ="",OFFSET(A12,-2,0)+1,OFFSET(A12,-1,0)+1 )</f>
         <v>8</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1010,104 +1016,138 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="13" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <f t="shared" ref="A16:A22" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
+      <c r="B13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="8"/>
+      <c r="B14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <f t="shared" ca="1" si="1"/>
+      <c r="A17" s="7">
         <v>11</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1119,11 +1159,11 @@
     </row>
     <row r="18" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ref="A18:A26" ca="1" si="2">IF(OFFSET(A18,-1,0) ="",OFFSET(A18,-2,0)+1,OFFSET(A18,-1,0)+1 )</f>
         <v>12</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1135,10 +1175,11 @@
     </row>
     <row r="19" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
-        <v>16</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1148,13 +1189,13 @@
       <c r="H19" s="4"/>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1164,13 +1205,13 @@
       <c r="H20" s="4"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1180,13 +1221,13 @@
       <c r="H21" s="4"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="25" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1194,69 +1235,80 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-    </row>
-    <row r="24" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
+        <f t="shared" ca="1" si="2"/>
         <v>18</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>19</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -1271,7 +1323,6 @@
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
-      <c r="B28" s="16"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1291,7 +1342,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="16"/>
       <c r="C30" s="4"/>
@@ -1300,9 +1351,9 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="16"/>
       <c r="C31" s="4"/>
@@ -1311,9 +1362,9 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="16"/>
       <c r="C32" s="4"/>
@@ -1335,11 +1386,27 @@
       <c r="H33" s="4"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-    </row>
-    <row r="35" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+    <row r="34" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
@@ -4290,14 +4357,20 @@
     <row r="1018" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1018" s="11"/>
     </row>
+    <row r="1019" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1019" s="11"/>
+    </row>
+    <row r="1020" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1020" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A25:I25"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A15:I15"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added original + discounted price and changed boundary values
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/Pham Hong Anh_Middle Assignment 1.xlsx
+++ b/Middle Assignment 1/Pham Hong Anh_Middle Assignment 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B9CB45-5ED5-47AE-B620-65698B8204FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8150E3D4-DC6E-4480-B833-A0899079F397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <author>ADMIN</author>
   </authors>
   <commentList>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{49865CBD-780A-45DC-B325-3B9CCFE0DD01}">
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{49865CBD-780A-45DC-B325-3B9CCFE0DD01}">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -100,22 +100,34 @@
     <t>2. View product function - Photo display</t>
   </si>
   <si>
-    <t>Verify that the &lt;&gt; button can help users navigate between photo using boundary value analysis with 2 boundary values of 1 and 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that discounted price is rounded to the nearest integer </t>
   </si>
   <si>
-    <t>Verify that commas are used as decimal separators to display price between ₫1,000 and ₫1,000,000</t>
+    <t>Verify that the maximum number of photos in the photo list is between 1 and 5</t>
   </si>
   <si>
-    <t>Verify that commas are used as decimal separators to display price between ₫0 and ₫1,000</t>
+    <t>Verify that 1 commas are used as decimal separators to display price between ₫1,000 and ₫999,999</t>
   </si>
   <si>
-    <t>Verify that commas are used as decimal separators to display price between ₫1,000 and ₫1,000,000,000</t>
+    <t>Verify that 2 commas are used as decimal separators to display price between ₫1,000,000 and ₫999,999,999</t>
   </si>
   <si>
-    <t>Verify that the maximum number of photos in the photo list is between 1 and 5</t>
+    <t>Verify that 0 comma is used as a decimal separator to display price between ₫0 and ₫999</t>
+  </si>
+  <si>
+    <t>Verify that 3 commas are used as decimal separators to display price between ₫1,000,000,000 and ₫999,999,999,999</t>
+  </si>
+  <si>
+    <t>Verify that the &gt; button navigates users to the next product photo but does not go above the 5th photo</t>
+  </si>
+  <si>
+    <t>Verify that the &lt; button navigates users to the previous product photo but does not go above the 1st photo</t>
+  </si>
+  <si>
+    <t>Original price</t>
+  </si>
+  <si>
+    <t>Discounted price</t>
   </si>
 </sst>
 </file>
@@ -176,7 +188,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +211,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8EB63E"/>
         <bgColor rgb="FF8EB63E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF8EB63E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -266,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -305,6 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -318,9 +345,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +567,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -601,17 +629,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -630,45 +658,42 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
+    <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
-        <f t="shared" ref="A4:A5" ca="1" si="0">IF(OFFSET(A4,-1,0) ="",OFFSET(A4,-2,0)+1,OFFSET(A4,-1,0)+1 )</f>
-        <v>2</v>
-      </c>
       <c r="B4" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -697,11 +722,11 @@
     </row>
     <row r="5" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="A5:A7" ca="1" si="0">IF(OFFSET(A5,-1,0) ="",OFFSET(A5,-2,0)+1,OFFSET(A5,-1,0)+1 )</f>
+        <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -728,13 +753,13 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
-        <f t="shared" ref="A6" ca="1" si="1">IF(OFFSET(A6,-1,0) ="",OFFSET(A6,-2,0)+1,OFFSET(A6,-1,0)+1 )</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -761,58 +786,75 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
+    <row r="7" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" ht="25" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" ht="25" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <f t="shared" ref="A9:A10" ca="1" si="2">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
-        <v>2</v>
-      </c>
       <c r="B9" s="13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -820,136 +862,330 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="8"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="A10:A12" ca="1" si="1">IF(OFFSET(A10,-1,0) ="",OFFSET(A10,-2,0)+1,OFFSET(A10,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>12</v>
+      <c r="B11" s="13" t="s">
+        <v>15</v>
       </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="13"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="13"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" ht="25" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <f t="shared" ref="A13" ca="1" si="2">IF(OFFSET(A13,-1,0) ="",OFFSET(A13,-2,0)+1,OFFSET(A13,-1,0)+1 )</f>
+        <v>5</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="13"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+    </row>
+    <row r="14" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="13"/>
+    <row r="16" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <f t="shared" ref="A16:A18" ca="1" si="3">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="13"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="13"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="7"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="7"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="7"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
@@ -3885,10 +4121,33 @@
     <row r="1004" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1004" s="9"/>
     </row>
+    <row r="1005" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1005" s="9"/>
+    </row>
+    <row r="1006" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1006" s="9"/>
+    </row>
+    <row r="1007" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1007" s="9"/>
+    </row>
+    <row r="1008" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1008" s="9"/>
+    </row>
+    <row r="1009" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1009" s="9"/>
+    </row>
+    <row r="1010" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1010" s="9"/>
+    </row>
+    <row r="1011" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1011" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Reworded the description of photos and buttons
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/Pham Hong Anh_Middle Assignment 1.xlsx
+++ b/Middle Assignment 1/Pham Hong Anh_Middle Assignment 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8150E3D4-DC6E-4480-B833-A0899079F397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1690CE0-E0A7-4A1A-8125-219286E3381D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <author>ADMIN</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{49865CBD-780A-45DC-B325-3B9CCFE0DD01}">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{49865CBD-780A-45DC-B325-3B9CCFE0DD01}">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -103,9 +103,6 @@
     <t xml:space="preserve">Verify that discounted price is rounded to the nearest integer </t>
   </si>
   <si>
-    <t>Verify that the maximum number of photos in the photo list is between 1 and 5</t>
-  </si>
-  <si>
     <t>Verify that 1 commas are used as decimal separators to display price between ₫1,000 and ₫999,999</t>
   </si>
   <si>
@@ -118,16 +115,28 @@
     <t>Verify that 3 commas are used as decimal separators to display price between ₫1,000,000,000 and ₫999,999,999,999</t>
   </si>
   <si>
-    <t>Verify that the &gt; button navigates users to the next product photo but does not go above the 5th photo</t>
-  </si>
-  <si>
-    <t>Verify that the &lt; button navigates users to the previous product photo but does not go above the 1st photo</t>
-  </si>
-  <si>
     <t>Original price</t>
   </si>
   <si>
     <t>Discounted price</t>
+  </si>
+  <si>
+    <t>Photos</t>
+  </si>
+  <si>
+    <t>Verify that there could be up to 5 photos in the photo list</t>
+  </si>
+  <si>
+    <t>Verify that the number of photos in the photo list could be higher than 5</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Verify that the &gt; button can navigate users to the next photo or from the 1st product photo to the last photo</t>
+  </si>
+  <si>
+    <t>Verify that the &lt; button can navigate users to the previous product photo or from the last photo to the 1st photo</t>
   </si>
 </sst>
 </file>
@@ -567,10 +576,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1011"/>
+  <dimension ref="A1:Z1014"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -660,7 +669,7 @@
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -693,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -726,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -759,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -792,7 +801,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -821,7 +830,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -854,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -887,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -920,7 +929,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -953,7 +962,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1043,54 +1052,74 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="25" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" ht="25" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" ht="25" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <f t="shared" ref="A16:A18" ca="1" si="3">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
-        <v>2</v>
-      </c>
       <c r="B16" s="13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="A16:A17" ca="1" si="3">IF(OFFSET(A17,-1,0) ="",OFFSET(A17,-2,0)+1,OFFSET(A17,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <f t="shared" ref="A18:A21" ca="1" si="4">IF(OFFSET(A18,-1,0) ="",OFFSET(A18,-2,0)+1,OFFSET(A18,-1,0)+1 )</f>
         <v>3</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
       <c r="B18" s="13" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1100,30 +1129,36 @@
       <c r="H18" s="3"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="13"/>
+    <row r="19" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1134,7 +1169,6 @@
     </row>
     <row r="22" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="13"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1143,7 +1177,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="13"/>
       <c r="C23" s="3"/>
@@ -1152,9 +1186,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="13"/>
       <c r="C24" s="3"/>
@@ -1163,9 +1197,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="13"/>
       <c r="C25" s="3"/>
@@ -1174,9 +1208,9 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="13"/>
       <c r="C26" s="3"/>
@@ -1187,14 +1221,38 @@
       <c r="H26" s="3"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+    <row r="27" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="7"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="7"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="7"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
@@ -4142,12 +4200,23 @@
     <row r="1011" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1011" s="9"/>
     </row>
+    <row r="1012" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1012" s="9"/>
+    </row>
+    <row r="1013" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1013" s="9"/>
+    </row>
+    <row r="1014" spans="1:1" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A1014" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A19:I19"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A14:I14"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>